<commit_message>
Alert window handling got added
</commit_message>
<xml_diff>
--- a/src/com/selenium/data/usrInfo.xlsx
+++ b/src/com/selenium/data/usrInfo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>frstName</t>
   </si>
@@ -91,9 +91,6 @@
     <t>male</t>
   </si>
   <si>
-    <t>11/31/1992</t>
-  </si>
-  <si>
     <t>music</t>
   </si>
   <si>
@@ -104,6 +101,54 @@
   </si>
   <si>
     <t>Agra</t>
+  </si>
+  <si>
+    <t>Shemshinur</t>
+  </si>
+  <si>
+    <t>Idris</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Sports, Reading</t>
+  </si>
+  <si>
+    <t>Amine</t>
+  </si>
+  <si>
+    <t>Abdurahman</t>
+  </si>
+  <si>
+    <t>Sports, Reading, Music</t>
+  </si>
+  <si>
+    <t>Sanuber</t>
+  </si>
+  <si>
+    <t>Rozi</t>
+  </si>
+  <si>
+    <t>Music, Reading</t>
+  </si>
+  <si>
+    <t>Mahire</t>
+  </si>
+  <si>
+    <t>Yaqup</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>Aygul</t>
+  </si>
+  <si>
+    <t>Omer</t>
+  </si>
+  <si>
+    <t>Sports</t>
   </si>
 </sst>
 </file>
@@ -367,6 +412,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="18.14"/>
+    <col customWidth="1" min="8" max="8" width="30.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -460,26 +509,216 @@
       <c r="E3" s="1">
         <v>6.044566666E9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
+      <c r="F3" s="2">
+        <v>31476.0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.343454567E9</v>
+      </c>
+      <c r="F4" s="2">
+        <v>33340.0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.044566666E9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>38751.0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.343454567E9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>35705.0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.044566666E9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>37144.0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.343454567E9</v>
+      </c>
+      <c r="F8" s="2">
+        <v>33032.0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>